<commit_message>
update 1 voor vv
</commit_message>
<xml_diff>
--- a/3-extraregels/IMKL-ExtraRegels-3.0.xlsx
+++ b/3-extraregels/IMKL-ExtraRegels-3.0.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28623"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\p.janssen.GNM\Documents\Github\imkl-werkomgeving\3-extraregels\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EAF1AE66-60CA-4531-9798-EB9B956D0AB6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC7DF07A-2E0C-471B-9EC4-DC500BC707DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-8010" windowWidth="29040" windowHeight="15720" tabRatio="875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="875" firstSheet="30" activeTab="34" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="NL-WIBON" sheetId="27" r:id="rId1"/>
@@ -70,7 +70,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4462" uniqueCount="456">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4463" uniqueCount="456">
   <si>
     <t>Annotatie</t>
   </si>
@@ -1487,21 +1487,6 @@
     </r>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>alle situaties: maximaal 1 algemene bijlage.
-uitlevering: afwezig indien beheerdersinformatieGeleverd=nee
-NietBetrokken: eisVoorzorgsmaatregelBijlage afwezig
-EisVoorzorgsmaatregel=ja dan bijlage verplicht en minstens 1 van type EisVoorzorgsmaatregelBijlage</t>
-    </r>
-  </si>
-  <si>
     <t>aanlegmethodeGestuurdeBoring</t>
   </si>
   <si>
@@ -1573,9 +1558,13 @@
     <t>Niet van toepassing als eigenaar = ja</t>
   </si>
   <si>
-    <t>Strikte verplichting IMKL.
-nilReason is niet toegestaan.
+    <t>Verplicht. nilReason mag.
 De UOM wordt uitgedrukt met urn:ogc:def:uom:OGC::bar</t>
+  </si>
+  <si>
+    <t>uitlevering: afwezig indien beheerdersinformatieGeleverd=nee
+NietBetrokken: eisVoorzorgsmaatregelBijlage afwezig
+EisVoorzorgsmaatregel=ja dan bijlage verplicht en minstens 1 van type EisVoorzorgsmaatregelBijlage</t>
   </si>
 </sst>
 </file>
@@ -2847,7 +2836,7 @@
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
-            <a:t> 3.0 </a:t>
+            <a:t> 3.0 Vastgestelde versie: </a:t>
           </a:r>
           <a:r>
             <a:rPr lang="nl-NL" sz="1100" baseline="0">
@@ -2858,7 +2847,7 @@
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
-            <a:t>2025-03-17 (hoort bij Informatiemodel Kabels en Leidingen (IMKL) versie 3.0 en </a:t>
+            <a:t>2025-06-16 (hoort bij Informatiemodel Kabels en Leidingen (IMKL) versie 3.0 en </a:t>
           </a:r>
           <a:endParaRPr lang="nl-NL"/>
         </a:p>
@@ -3369,7 +3358,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="Q19" sqref="Q19"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <sheetData/>
@@ -3886,7 +3877,7 @@
         <v>29</v>
       </c>
       <c r="F25" s="20" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.3">
@@ -3911,7 +3902,7 @@
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A27" s="20" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="B27" s="20" t="s">
         <v>81</v>
@@ -3931,13 +3922,13 @@
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A28" s="20" t="s">
+        <v>436</v>
+      </c>
+      <c r="B28" s="20" t="s">
         <v>437</v>
       </c>
-      <c r="B28" s="20" t="s">
-        <v>438</v>
-      </c>
       <c r="C28" s="34" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="D28" s="35" t="s">
         <v>54</v>
@@ -3951,13 +3942,13 @@
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A29" s="20" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="B29" s="20" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="C29" s="34" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="D29" s="35" t="s">
         <v>54</v>
@@ -3971,13 +3962,13 @@
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A30" s="20" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="B30" s="20" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="C30" s="34" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="D30" s="35" t="s">
         <v>54</v>
@@ -3991,13 +3982,13 @@
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A31" s="20" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="B31" s="20" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="C31" s="34" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="D31" s="35" t="s">
         <v>54</v>
@@ -4011,13 +4002,13 @@
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A32" s="20" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="B32" s="20" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="C32" s="34" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="D32" s="35" t="s">
         <v>54</v>
@@ -4031,13 +4022,13 @@
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A33" s="20" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="B33" s="20" t="s">
+        <v>442</v>
+      </c>
+      <c r="C33" s="34" t="s">
         <v>443</v>
-      </c>
-      <c r="C33" s="34" t="s">
-        <v>444</v>
       </c>
       <c r="D33" s="35" t="s">
         <v>54</v>
@@ -4111,7 +4102,7 @@
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="B37" t="s">
         <v>81</v>
@@ -4761,7 +4752,7 @@
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A32" s="20" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B32" s="34" t="s">
         <v>81</v>
@@ -4781,7 +4772,7 @@
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A33" s="20" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B33" s="34" t="s">
         <v>81</v>
@@ -4796,7 +4787,7 @@
         <v>29</v>
       </c>
       <c r="F33" s="21" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
     </row>
   </sheetData>
@@ -8093,7 +8084,7 @@
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22" s="20" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="B22" s="20" t="s">
         <v>81</v>
@@ -8939,7 +8930,7 @@
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22" s="21" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B22" s="21" t="s">
         <v>125</v>
@@ -8959,7 +8950,7 @@
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23" s="21" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B23" s="21" t="s">
         <v>125</v>
@@ -9218,7 +9209,7 @@
         <v>29</v>
       </c>
       <c r="F7" s="20" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -9238,7 +9229,7 @@
         <v>29</v>
       </c>
       <c r="F8" s="30" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
@@ -12329,7 +12320,7 @@
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21" s="21" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B21" s="21" t="s">
         <v>125</v>
@@ -12349,7 +12340,7 @@
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22" s="21" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B22" s="21" t="s">
         <v>125</v>
@@ -13418,7 +13409,7 @@
         <v>29</v>
       </c>
       <c r="F34" s="20" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.3">
@@ -14176,15 +14167,15 @@
         <v>29</v>
       </c>
       <c r="F61" s="52" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
     </row>
     <row r="62" spans="1:115" x14ac:dyDescent="0.3">
       <c r="A62" s="20" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="B62" s="20" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="C62" s="20" t="s">
         <v>274</v>
@@ -14201,10 +14192,10 @@
     </row>
     <row r="63" spans="1:115" x14ac:dyDescent="0.3">
       <c r="A63" s="20" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="B63" s="20" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="C63" s="20" t="s">
         <v>274</v>
@@ -14221,10 +14212,10 @@
     </row>
     <row r="64" spans="1:115" x14ac:dyDescent="0.3">
       <c r="A64" s="20" t="s">
+        <v>448</v>
+      </c>
+      <c r="B64" s="20" t="s">
         <v>449</v>
-      </c>
-      <c r="B64" s="20" t="s">
-        <v>450</v>
       </c>
       <c r="C64" s="20" t="s">
         <v>274</v>
@@ -15162,10 +15153,13 @@
 
 <file path=xl/worksheets/sheet35.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2000-000000000000}">
+  <sheetPr>
+    <tabColor rgb="FF92D050"/>
+  </sheetPr>
   <dimension ref="A1:F15"/>
   <sheetViews>
-    <sheetView topLeftCell="A9" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="A29" sqref="A29"/>
+    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -15423,8 +15417,8 @@
       <c r="E13" s="33" t="s">
         <v>35</v>
       </c>
-      <c r="F13" s="25" t="s">
-        <v>431</v>
+      <c r="F13" s="26" t="s">
+        <v>455</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="46.8" x14ac:dyDescent="0.3">
@@ -16988,7 +16982,7 @@
   </sheetPr>
   <dimension ref="A1:F30"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" zoomScaleNormal="100" zoomScaleSheetLayoutView="125" zoomScalePageLayoutView="125" workbookViewId="0">
+    <sheetView topLeftCell="A10" zoomScaleNormal="100" zoomScaleSheetLayoutView="125" zoomScalePageLayoutView="125" workbookViewId="0">
       <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
@@ -17329,8 +17323,8 @@
       <c r="E17" s="24" t="s">
         <v>29</v>
       </c>
-      <c r="F17" s="24" t="s">
-        <v>455</v>
+      <c r="F17" s="21" t="s">
+        <v>454</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.3">
@@ -17475,7 +17469,7 @@
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A25" s="21" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B25" s="21" t="s">
         <v>125</v>
@@ -17495,7 +17489,7 @@
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A26" s="21" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B26" s="21" t="s">
         <v>125</v>
@@ -17614,8 +17608,8 @@
   </sheetPr>
   <dimension ref="A1:F30"/>
   <sheetViews>
-    <sheetView topLeftCell="A11" zoomScaleNormal="100" zoomScaleSheetLayoutView="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="A18" sqref="A18:XFD18"/>
+    <sheetView topLeftCell="A8" zoomScaleNormal="100" zoomScaleSheetLayoutView="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.69921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -17952,7 +17946,7 @@
         <v>29</v>
       </c>
       <c r="F17" s="21" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.3">
@@ -18097,7 +18091,7 @@
     </row>
     <row r="25" spans="1:6" s="24" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A25" s="21" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B25" s="21" t="s">
         <v>125</v>
@@ -18117,7 +18111,7 @@
     </row>
     <row r="26" spans="1:6" s="24" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A26" s="21" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B26" s="21" t="s">
         <v>125</v>
@@ -18237,7 +18231,7 @@
   <dimension ref="A1:F30"/>
   <sheetViews>
     <sheetView topLeftCell="A16" zoomScaleNormal="100" zoomScaleSheetLayoutView="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17:XFD17"/>
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -18561,7 +18555,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="17" spans="1:6" s="24" customFormat="1" ht="46.8" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:6" s="24" customFormat="1" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A17" s="24" t="s">
         <v>63</v>
       </c>
@@ -18578,7 +18572,7 @@
         <v>29</v>
       </c>
       <c r="F17" s="21" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.3">
@@ -18723,7 +18717,7 @@
     </row>
     <row r="25" spans="1:6" s="24" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A25" s="21" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B25" s="21" t="s">
         <v>125</v>
@@ -18743,7 +18737,7 @@
     </row>
     <row r="26" spans="1:6" s="24" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A26" s="21" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B26" s="21" t="s">
         <v>125</v>
@@ -18863,7 +18857,7 @@
   <dimension ref="A1:F28"/>
   <sheetViews>
     <sheetView topLeftCell="A13" zoomScaleNormal="100" zoomScaleSheetLayoutView="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="A18" sqref="A17:XFD18"/>
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -19187,7 +19181,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="17" spans="1:6" ht="46.8" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:6" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A17" s="24" t="s">
         <v>63</v>
       </c>
@@ -19204,7 +19198,7 @@
         <v>29</v>
       </c>
       <c r="F17" s="21" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.3">
@@ -19349,7 +19343,7 @@
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A25" s="21" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B25" s="21" t="s">
         <v>125</v>
@@ -19369,7 +19363,7 @@
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A26" s="21" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B26" s="21" t="s">
         <v>125</v>
@@ -19448,7 +19442,7 @@
   <dimension ref="A1:F29"/>
   <sheetViews>
     <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="D25" sqref="D25"/>
+      <selection activeCell="F26" sqref="F26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -19833,7 +19827,7 @@
     </row>
     <row r="20" spans="1:6" s="24" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A20" s="21" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B20" s="21" t="s">
         <v>125</v>
@@ -19853,7 +19847,7 @@
     </row>
     <row r="21" spans="1:6" s="24" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A21" s="21" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B21" s="21" t="s">
         <v>125</v>
@@ -19941,8 +19935,8 @@
       <c r="C25" s="32" t="s">
         <v>274</v>
       </c>
-      <c r="D25" s="35">
-        <v>1</v>
+      <c r="D25" s="31" t="s">
+        <v>54</v>
       </c>
       <c r="E25" t="s">
         <v>29</v>
@@ -20540,7 +20534,7 @@
         <v>29</v>
       </c>
       <c r="F25" s="20" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.3">

</xml_diff>